<commit_message>
commit all: finished ach loop
</commit_message>
<xml_diff>
--- a/Achievement_Hunting/achievement_hunting_venv/achievement_hunting.xlsx
+++ b/Achievement_Hunting/achievement_hunting_venv/achievement_hunting.xlsx
@@ -7027,7 +7027,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E252"/>
+  <dimension ref="A1:G252"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -7061,6 +7061,16 @@
           <t>TA-Ratio</t>
         </is>
       </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>Total Diff</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>Diff Left</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2">
@@ -7083,6 +7093,12 @@
         <f>'Game'!E2/'Game'!G2</f>
         <v/>
       </c>
+      <c r="F2" t="n">
+        <v>0.1558942792840858</v>
+      </c>
+      <c r="G2" t="n">
+        <v>0.001202585393733075</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3">
@@ -7105,6 +7121,12 @@
         <f>'Game'!E3/'Game'!G3</f>
         <v/>
       </c>
+      <c r="F3" t="n">
+        <v>0.2393526372830986</v>
+      </c>
+      <c r="G3" t="n">
+        <v>8.606923059812515e-06</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4">
@@ -7127,6 +7149,12 @@
         <f>'Game'!E4/'Game'!G4</f>
         <v/>
       </c>
+      <c r="F4" t="n">
+        <v>0.1771739584375805</v>
+      </c>
+      <c r="G4" t="n">
+        <v>3.772351277962694e-06</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5">
@@ -7149,6 +7177,12 @@
         <f>'Game'!E5/'Game'!G5</f>
         <v/>
       </c>
+      <c r="F5" t="n">
+        <v>0.3300473061752675</v>
+      </c>
+      <c r="G5" t="n">
+        <v>8.685098749162529e-06</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6">
@@ -7171,6 +7205,12 @@
         <f>'Game'!E6/'Game'!G6</f>
         <v/>
       </c>
+      <c r="F6" t="n">
+        <v>0.4492233826161332</v>
+      </c>
+      <c r="G6" t="n">
+        <v>0.000187858283317944</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7">
@@ -7193,6 +7233,12 @@
         <f>'Game'!E7/'Game'!G7</f>
         <v/>
       </c>
+      <c r="F7" t="n">
+        <v>0.06557796318125259</v>
+      </c>
+      <c r="G7" t="n">
+        <v>8.200969262305901e-07</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8">
@@ -7215,6 +7261,12 @@
         <f>'Game'!E8/'Game'!G8</f>
         <v/>
       </c>
+      <c r="F8" t="n">
+        <v>0.05583527788994465</v>
+      </c>
+      <c r="G8" t="n">
+        <v>0.002240817898532965</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9">
@@ -7237,6 +7289,12 @@
         <f>'Game'!E9/'Game'!G9</f>
         <v/>
       </c>
+      <c r="F9" t="n">
+        <v>0.299978773614354</v>
+      </c>
+      <c r="G9" t="n">
+        <v>2.417579468196838e-05</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10">
@@ -7259,6 +7317,12 @@
         <f>'Game'!E10/'Game'!G10</f>
         <v/>
       </c>
+      <c r="F10" t="n">
+        <v>0.09306408281065442</v>
+      </c>
+      <c r="G10" t="n">
+        <v>7.945001482015885e-06</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11">
@@ -7281,6 +7345,12 @@
         <f>'Game'!E11/'Game'!G11</f>
         <v/>
       </c>
+      <c r="F11" t="n">
+        <v>0.1204795906970961</v>
+      </c>
+      <c r="G11" t="n">
+        <v>2.711845561751181e-06</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12">
@@ -7303,6 +7373,12 @@
         <f>'Game'!E12/'Game'!G12</f>
         <v/>
       </c>
+      <c r="F12" t="n">
+        <v>0.2648831904862434</v>
+      </c>
+      <c r="G12" t="n">
+        <v>2.834177918353003e-06</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13">
@@ -7325,6 +7401,12 @@
         <f>'Game'!E13/'Game'!G13</f>
         <v/>
       </c>
+      <c r="F13" t="n">
+        <v>0.1699097914935002</v>
+      </c>
+      <c r="G13" t="n">
+        <v>1.918340098679415e-06</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14">
@@ -7347,6 +7429,12 @@
         <f>'Game'!E14/'Game'!G14</f>
         <v/>
       </c>
+      <c r="F14" t="n">
+        <v>0.09520109374632582</v>
+      </c>
+      <c r="G14" t="n">
+        <v>0.0002409675483219453</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15">
@@ -7369,6 +7457,12 @@
         <f>'Game'!E15/'Game'!G15</f>
         <v/>
       </c>
+      <c r="F15" t="n">
+        <v>0.1186604328803788</v>
+      </c>
+      <c r="G15" t="n">
+        <v>4.914240966611541e-05</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16">
@@ -7391,6 +7485,12 @@
         <f>'Game'!E16/'Game'!G16</f>
         <v/>
       </c>
+      <c r="F16" t="n">
+        <v>0.1628536121908306</v>
+      </c>
+      <c r="G16" t="n">
+        <v>0.0004151364736248854</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17">
@@ -7413,6 +7513,12 @@
         <f>'Game'!E17/'Game'!G17</f>
         <v/>
       </c>
+      <c r="F17" t="n">
+        <v>0.1506982755294934</v>
+      </c>
+      <c r="G17" t="n">
+        <v>0.001512849920295502</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18">
@@ -7435,6 +7541,12 @@
         <f>'Game'!E18/'Game'!G18</f>
         <v/>
       </c>
+      <c r="F18" t="n">
+        <v>0.1644424185138483</v>
+      </c>
+      <c r="G18" t="n">
+        <v>2.472912164654338e-06</v>
+      </c>
     </row>
     <row r="19">
       <c r="A19">
@@ -7457,6 +7569,12 @@
         <f>'Game'!E19/'Game'!G19</f>
         <v/>
       </c>
+      <c r="F19" t="n">
+        <v>0.7037971262555741</v>
+      </c>
+      <c r="G19" t="n">
+        <v>1.516386681029881e-05</v>
+      </c>
     </row>
     <row r="20">
       <c r="A20">
@@ -7479,6 +7597,12 @@
         <f>'Game'!E20/'Game'!G20</f>
         <v/>
       </c>
+      <c r="F20" t="n">
+        <v>0.365093418278402</v>
+      </c>
+      <c r="G20" t="n">
+        <v>2.162627362011534e-05</v>
+      </c>
     </row>
     <row r="21">
       <c r="A21">
@@ -7501,6 +7625,12 @@
         <f>'Game'!E21/'Game'!G21</f>
         <v/>
       </c>
+      <c r="F21" t="n">
+        <v>0.4036366043505568</v>
+      </c>
+      <c r="G21" t="n">
+        <v>5.333646240579448e-06</v>
+      </c>
     </row>
     <row r="22">
       <c r="A22">
@@ -7523,6 +7653,12 @@
         <f>'Game'!E22/'Game'!G22</f>
         <v/>
       </c>
+      <c r="F22" t="n">
+        <v>0.3069344157887063</v>
+      </c>
+      <c r="G22" t="n">
+        <v>3.487754700419456e-06</v>
+      </c>
     </row>
     <row r="23">
       <c r="A23">
@@ -7545,6 +7681,12 @@
         <f>'Game'!E23/'Game'!G23</f>
         <v/>
       </c>
+      <c r="F23" t="n">
+        <v>0.07881559703918177</v>
+      </c>
+      <c r="G23" t="n">
+        <v>8.648900537357864e-07</v>
+      </c>
     </row>
     <row r="24">
       <c r="A24">
@@ -7567,6 +7709,12 @@
         <f>'Game'!E24/'Game'!G24</f>
         <v/>
       </c>
+      <c r="F24" t="n">
+        <v>0.03655919482029327</v>
+      </c>
+      <c r="G24" t="n">
+        <v>4.246843082651742e-05</v>
+      </c>
     </row>
     <row r="25">
       <c r="A25">
@@ -7589,6 +7737,12 @@
         <f>'Game'!E25/'Game'!G25</f>
         <v/>
       </c>
+      <c r="F25" t="n">
+        <v>0.02303588635830065</v>
+      </c>
+      <c r="G25" t="n">
+        <v>1.900813000952666e-05</v>
+      </c>
     </row>
     <row r="26">
       <c r="A26">
@@ -7611,6 +7765,12 @@
         <f>'Game'!E26/'Game'!G26</f>
         <v/>
       </c>
+      <c r="F26" t="n">
+        <v>0.01273316915694349</v>
+      </c>
+      <c r="G26" t="n">
+        <v>5.679676653281884e-05</v>
+      </c>
     </row>
     <row r="27">
       <c r="A27">
@@ -7633,6 +7793,12 @@
         <f>'Game'!E27/'Game'!G27</f>
         <v/>
       </c>
+      <c r="F27" t="n">
+        <v>0.2571497928401269</v>
+      </c>
+      <c r="G27" t="n">
+        <v>0.0001098761037054617</v>
+      </c>
     </row>
     <row r="28">
       <c r="A28">
@@ -7655,6 +7821,12 @@
         <f>'Game'!E28/'Game'!G28</f>
         <v/>
       </c>
+      <c r="F28" t="n">
+        <v>0.008101620243032405</v>
+      </c>
+      <c r="G28" t="n">
+        <v>3.287230987089475e-06</v>
+      </c>
     </row>
     <row r="29">
       <c r="A29">
@@ -7677,6 +7849,12 @@
         <f>'Game'!E29/'Game'!G29</f>
         <v/>
       </c>
+      <c r="F29" t="n">
+        <v>0.01996648465818247</v>
+      </c>
+      <c r="G29" t="n">
+        <v>1.650375152696681e-05</v>
+      </c>
     </row>
     <row r="30">
       <c r="A30">
@@ -7699,6 +7877,12 @@
         <f>'Game'!E30/'Game'!G30</f>
         <v/>
       </c>
+      <c r="F30" t="n">
+        <v>0.07444782975270292</v>
+      </c>
+      <c r="G30" t="n">
+        <v>1.858147523199285e-05</v>
+      </c>
     </row>
     <row r="31">
       <c r="A31">
@@ -7721,6 +7905,12 @@
         <f>'Game'!E31/'Game'!G31</f>
         <v/>
       </c>
+      <c r="F31" t="n">
+        <v>0.0440601947088393</v>
+      </c>
+      <c r="G31" t="n">
+        <v>1.52659331404758e-05</v>
+      </c>
     </row>
     <row r="32">
       <c r="A32">
@@ -7743,6 +7933,12 @@
         <f>'Game'!E32/'Game'!G32</f>
         <v/>
       </c>
+      <c r="F32" t="n">
+        <v>0.2657030502710171</v>
+      </c>
+      <c r="G32" t="n">
+        <v>2.639549274092394e-06</v>
+      </c>
     </row>
     <row r="33">
       <c r="A33">
@@ -7765,6 +7961,12 @@
         <f>'Game'!E33/'Game'!G33</f>
         <v/>
       </c>
+      <c r="F33" t="n">
+        <v>0.2250395169391745</v>
+      </c>
+      <c r="G33" t="n">
+        <v>9.817917409884471e-06</v>
+      </c>
     </row>
     <row r="34">
       <c r="A34">
@@ -7787,6 +7989,12 @@
         <f>'Game'!E34/'Game'!G34</f>
         <v/>
       </c>
+      <c r="F34" t="n">
+        <v>0.8130867945760606</v>
+      </c>
+      <c r="G34" t="n">
+        <v>1.375815583477885e-05</v>
+      </c>
     </row>
     <row r="35">
       <c r="A35">
@@ -7809,6 +8017,12 @@
         <f>'Game'!E35/'Game'!G35</f>
         <v/>
       </c>
+      <c r="F35" t="n">
+        <v>0.4665711129027442</v>
+      </c>
+      <c r="G35" t="n">
+        <v>4.386702136824235e-05</v>
+      </c>
     </row>
     <row r="36">
       <c r="A36">
@@ -7831,6 +8045,12 @@
         <f>'Game'!E36/'Game'!G36</f>
         <v/>
       </c>
+      <c r="F36" t="n">
+        <v>0.3131489032429388</v>
+      </c>
+      <c r="G36" t="n">
+        <v>9.538347409640139e-06</v>
+      </c>
     </row>
     <row r="37">
       <c r="A37">
@@ -7853,6 +8073,12 @@
         <f>'Game'!E37/'Game'!G37</f>
         <v/>
       </c>
+      <c r="F37" t="n">
+        <v>0.3042316492793209</v>
+      </c>
+      <c r="G37" t="n">
+        <v>3.819246184092864e-06</v>
+      </c>
     </row>
     <row r="38">
       <c r="A38">
@@ -7875,6 +8101,12 @@
         <f>'Game'!E38/'Game'!G38</f>
         <v/>
       </c>
+      <c r="F38" t="n">
+        <v>0.373166493082053</v>
+      </c>
+      <c r="G38" t="n">
+        <v>6.708113416220126e-06</v>
+      </c>
     </row>
     <row r="39">
       <c r="A39">
@@ -7897,6 +8129,12 @@
         <f>'Game'!E39/'Game'!G39</f>
         <v/>
       </c>
+      <c r="F39" t="n">
+        <v>0.1422920199362503</v>
+      </c>
+      <c r="G39" t="n">
+        <v>2.02056021042114e-06</v>
+      </c>
     </row>
     <row r="40">
       <c r="A40">
@@ -7919,6 +8157,12 @@
         <f>'Game'!E40/'Game'!G40</f>
         <v/>
       </c>
+      <c r="F40" t="n">
+        <v>0.2161320532264085</v>
+      </c>
+      <c r="G40" t="n">
+        <v>7.459837527170566e-06</v>
+      </c>
     </row>
     <row r="41">
       <c r="A41">
@@ -7941,6 +8185,12 @@
         <f>'Game'!E41/'Game'!G41</f>
         <v/>
       </c>
+      <c r="F41" t="n">
+        <v>0.07203014663321011</v>
+      </c>
+      <c r="G41" t="n">
+        <v>7.124784130440503e-06</v>
+      </c>
     </row>
     <row r="42">
       <c r="A42">
@@ -7963,6 +8213,12 @@
         <f>'Game'!E42/'Game'!G42</f>
         <v/>
       </c>
+      <c r="F42" t="n">
+        <v>0.2032716986440151</v>
+      </c>
+      <c r="G42" t="n">
+        <v>6.534348718849453e-06</v>
+      </c>
     </row>
     <row r="43">
       <c r="A43">
@@ -7985,6 +8241,12 @@
         <f>'Game'!E43/'Game'!G43</f>
         <v/>
       </c>
+      <c r="F43" t="n">
+        <v>0.08572985492674519</v>
+      </c>
+      <c r="G43" t="n">
+        <v>1.966836362619767e-08</v>
+      </c>
     </row>
     <row r="44">
       <c r="A44">
@@ -8007,6 +8269,12 @@
         <f>'Game'!E44/'Game'!G44</f>
         <v/>
       </c>
+      <c r="F44" t="n">
+        <v>0.1050726445996601</v>
+      </c>
+      <c r="G44" t="n">
+        <v>1.393019871906278e-05</v>
+      </c>
     </row>
     <row r="45">
       <c r="A45">
@@ -8029,6 +8297,12 @@
         <f>'Game'!E45/'Game'!G45</f>
         <v/>
       </c>
+      <c r="F45" t="n">
+        <v>0.02474890890052008</v>
+      </c>
+      <c r="G45" t="n">
+        <v>6.881596345212921e-07</v>
+      </c>
     </row>
     <row r="46">
       <c r="A46">
@@ -8051,6 +8325,12 @@
         <f>'Game'!E46/'Game'!G46</f>
         <v/>
       </c>
+      <c r="F46" t="n">
+        <v>0.3682015270053728</v>
+      </c>
+      <c r="G46" t="n">
+        <v>4.622426040887511e-06</v>
+      </c>
     </row>
     <row r="47">
       <c r="A47">
@@ -8073,6 +8353,12 @@
         <f>'Game'!E47/'Game'!G47</f>
         <v/>
       </c>
+      <c r="F47" t="n">
+        <v>0.1772355647343448</v>
+      </c>
+      <c r="G47" t="n">
+        <v>5.516843786085762e-06</v>
+      </c>
     </row>
     <row r="48">
       <c r="A48">
@@ -8095,6 +8381,12 @@
         <f>'Game'!E48/'Game'!G48</f>
         <v/>
       </c>
+      <c r="F48" t="n">
+        <v>0.1365665742930358</v>
+      </c>
+      <c r="G48" t="n">
+        <v>2.970775804049458e-05</v>
+      </c>
     </row>
     <row r="49">
       <c r="A49">
@@ -8117,6 +8409,12 @@
         <f>'Game'!E49/'Game'!G49</f>
         <v/>
       </c>
+      <c r="F49" t="n">
+        <v>0.07352214604674361</v>
+      </c>
+      <c r="G49" t="n">
+        <v>0.0003296189236069909</v>
+      </c>
     </row>
     <row r="50">
       <c r="A50">
@@ -8139,6 +8437,12 @@
         <f>'Game'!E50/'Game'!G50</f>
         <v/>
       </c>
+      <c r="F50" t="n">
+        <v>0.230252614748693</v>
+      </c>
+      <c r="G50" t="n">
+        <v>1.473164288359794e-05</v>
+      </c>
     </row>
     <row r="51">
       <c r="A51">
@@ -8161,6 +8465,12 @@
         <f>'Game'!E51/'Game'!G51</f>
         <v/>
       </c>
+      <c r="F51" t="n">
+        <v>0.06928854041680245</v>
+      </c>
+      <c r="G51" t="n">
+        <v>3.518703191791034e-06</v>
+      </c>
     </row>
     <row r="52">
       <c r="A52">
@@ -8183,6 +8493,12 @@
         <f>'Game'!E52/'Game'!G52</f>
         <v/>
       </c>
+      <c r="F52" t="n">
+        <v>0.1308005977587317</v>
+      </c>
+      <c r="G52" t="n">
+        <v>7.212372825582286e-05</v>
+      </c>
     </row>
     <row r="53">
       <c r="A53">
@@ -8205,6 +8521,12 @@
         <f>'Game'!E53/'Game'!G53</f>
         <v/>
       </c>
+      <c r="F53" t="n">
+        <v>0.1308005977587317</v>
+      </c>
+      <c r="G53" t="n">
+        <v>0.0003533269263384024</v>
+      </c>
     </row>
     <row r="54">
       <c r="A54">
@@ -8227,6 +8549,12 @@
         <f>'Game'!E54/'Game'!G54</f>
         <v/>
       </c>
+      <c r="F54" t="n">
+        <v>0.06234404248123054</v>
+      </c>
+      <c r="G54" t="n">
+        <v>8.251673779411424e-06</v>
+      </c>
     </row>
     <row r="55">
       <c r="A55">
@@ -8249,6 +8577,12 @@
         <f>'Game'!E55/'Game'!G55</f>
         <v/>
       </c>
+      <c r="F55" t="n">
+        <v>0.2300318018966122</v>
+      </c>
+      <c r="G55" t="n">
+        <v>7.014413216276806e-05</v>
+      </c>
     </row>
     <row r="56">
       <c r="A56">
@@ -8271,6 +8605,12 @@
         <f>'Game'!E56/'Game'!G56</f>
         <v/>
       </c>
+      <c r="F56" t="n">
+        <v>0.406731570179092</v>
+      </c>
+      <c r="G56" t="n">
+        <v>9.288264928184845e-06</v>
+      </c>
     </row>
     <row r="57">
       <c r="A57">
@@ -8293,6 +8633,12 @@
         <f>'Game'!E57/'Game'!G57</f>
         <v/>
       </c>
+      <c r="F57" t="n">
+        <v>0.09039731064384941</v>
+      </c>
+      <c r="G57" t="n">
+        <v>0.0001023402922173534</v>
+      </c>
     </row>
     <row r="58">
       <c r="A58">
@@ -8315,6 +8661,12 @@
         <f>'Game'!E58/'Game'!G58</f>
         <v/>
       </c>
+      <c r="F58" t="n">
+        <v>0.1042599684780411</v>
+      </c>
+      <c r="G58" t="n">
+        <v>1.548174008101363e-05</v>
+      </c>
     </row>
     <row r="59">
       <c r="A59">
@@ -8337,6 +8689,12 @@
         <f>'Game'!E59/'Game'!G59</f>
         <v/>
       </c>
+      <c r="F59" t="n">
+        <v>0.126105694731405</v>
+      </c>
+      <c r="G59" t="n">
+        <v>1.79045555397877e-06</v>
+      </c>
     </row>
     <row r="60">
       <c r="A60">
@@ -8359,6 +8717,12 @@
         <f>'Game'!E60/'Game'!G60</f>
         <v/>
       </c>
+      <c r="F60" t="n">
+        <v>0.1181714481001045</v>
+      </c>
+      <c r="G60" t="n">
+        <v>3.532982454474272e-05</v>
+      </c>
     </row>
     <row r="61">
       <c r="A61">
@@ -8381,6 +8745,12 @@
         <f>'Game'!E61/'Game'!G61</f>
         <v/>
       </c>
+      <c r="F61" t="n">
+        <v>0.5446548930433954</v>
+      </c>
+      <c r="G61" t="n">
+        <v>6.298815822625347e-05</v>
+      </c>
     </row>
     <row r="62">
       <c r="A62">
@@ -8403,6 +8773,12 @@
         <f>'Game'!E62/'Game'!G62</f>
         <v/>
       </c>
+      <c r="F62" t="n">
+        <v>0.3881949903436496</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.0001792085790730974</v>
+      </c>
     </row>
     <row r="63">
       <c r="A63">
@@ -8425,6 +8801,12 @@
         <f>'Game'!E63/'Game'!G63</f>
         <v/>
       </c>
+      <c r="F63" t="n">
+        <v>0.02679536947076546</v>
+      </c>
+      <c r="G63" t="n">
+        <v>1.347380132310546e-05</v>
+      </c>
     </row>
     <row r="64">
       <c r="A64">
@@ -8447,6 +8829,12 @@
         <f>'Game'!E64/'Game'!G64</f>
         <v/>
       </c>
+      <c r="F64" t="n">
+        <v>0.0179930465871464</v>
+      </c>
+      <c r="G64" t="n">
+        <v>4.531022497360408e-05</v>
+      </c>
     </row>
     <row r="65">
       <c r="A65">
@@ -8469,6 +8857,12 @@
         <f>'Game'!E65/'Game'!G65</f>
         <v/>
       </c>
+      <c r="F65" t="n">
+        <v>0.0177163080156603</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.0001777303798501665</v>
+      </c>
     </row>
     <row r="66">
       <c r="A66">
@@ -8491,6 +8885,12 @@
         <f>'Game'!E66/'Game'!G66</f>
         <v/>
       </c>
+      <c r="F66" t="n">
+        <v>0.01884260255910807</v>
+      </c>
+      <c r="G66" t="n">
+        <v>3.053253259476664e-05</v>
+      </c>
     </row>
     <row r="67">
       <c r="A67">
@@ -8513,6 +8913,12 @@
         <f>'Game'!E67/'Game'!G67</f>
         <v/>
       </c>
+      <c r="F67" t="n">
+        <v>0.01334952630874585</v>
+      </c>
+      <c r="G67" t="n">
+        <v>3.8158896379755e-06</v>
+      </c>
     </row>
     <row r="68">
       <c r="A68">
@@ -8535,6 +8941,12 @@
         <f>'Game'!E68/'Game'!G68</f>
         <v/>
       </c>
+      <c r="F68" t="n">
+        <v>0.1992984693877551</v>
+      </c>
+      <c r="G68" t="n">
+        <v>4.992679327914217e-05</v>
+      </c>
     </row>
     <row r="69">
       <c r="A69">
@@ -8557,6 +8969,12 @@
         <f>'Game'!E69/'Game'!G69</f>
         <v/>
       </c>
+      <c r="F69" t="n">
+        <v>0.1328103086299076</v>
+      </c>
+      <c r="G69" t="n">
+        <v>2.183386579378062e-06</v>
+      </c>
     </row>
     <row r="70">
       <c r="A70">
@@ -8579,6 +8997,12 @@
         <f>'Game'!E70/'Game'!G70</f>
         <v/>
       </c>
+      <c r="F70" t="n">
+        <v>0.009583480379860411</v>
+      </c>
+      <c r="G70" t="n">
+        <v>4.339667512033899e-05</v>
+      </c>
     </row>
     <row r="71">
       <c r="A71">
@@ -8601,6 +9025,12 @@
         <f>'Game'!E71/'Game'!G71</f>
         <v/>
       </c>
+      <c r="F71" t="n">
+        <v>0.02683049366096048</v>
+      </c>
+      <c r="G71" t="n">
+        <v>3.58659884828594e-06</v>
+      </c>
     </row>
     <row r="72">
       <c r="A72">
@@ -8623,6 +9053,12 @@
         <f>'Game'!E72/'Game'!G72</f>
         <v/>
       </c>
+      <c r="F72" t="n">
+        <v>0.04781868150601494</v>
+      </c>
+      <c r="G72" t="n">
+        <v>3.127049683347131e-06</v>
+      </c>
     </row>
     <row r="73">
       <c r="A73">
@@ -8645,6 +9081,12 @@
         <f>'Game'!E73/'Game'!G73</f>
         <v/>
       </c>
+      <c r="F73" t="n">
+        <v>0.42165626581211</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.0006676949168385982</v>
+      </c>
     </row>
     <row r="74">
       <c r="A74">
@@ -8667,6 +9109,12 @@
         <f>'Game'!E74/'Game'!G74</f>
         <v/>
       </c>
+      <c r="F74" t="n">
+        <v>0.4072508571612416</v>
+      </c>
+      <c r="G74" t="n">
+        <v>5.053500765758992e-06</v>
+      </c>
     </row>
     <row r="75">
       <c r="A75">
@@ -8689,6 +9137,12 @@
         <f>'Game'!E75/'Game'!G75</f>
         <v/>
       </c>
+      <c r="F75" t="n">
+        <v>0.02195437831885709</v>
+      </c>
+      <c r="G75" t="n">
+        <v>9.177663494803513e-07</v>
+      </c>
     </row>
     <row r="76">
       <c r="A76">
@@ -8711,6 +9165,12 @@
         <f>'Game'!E76/'Game'!G76</f>
         <v/>
       </c>
+      <c r="F76" t="n">
+        <v>0.1193171479622123</v>
+      </c>
+      <c r="G76" t="n">
+        <v>3.950543393767335e-06</v>
+      </c>
     </row>
     <row r="77">
       <c r="A77">
@@ -8733,6 +9193,12 @@
         <f>'Game'!E77/'Game'!G77</f>
         <v/>
       </c>
+      <c r="F77" t="n">
+        <v>0.1043947583391838</v>
+      </c>
+      <c r="G77" t="n">
+        <v>1.710713237940613e-05</v>
+      </c>
     </row>
     <row r="78">
       <c r="A78">
@@ -8755,6 +9221,12 @@
         <f>'Game'!E78/'Game'!G78</f>
         <v/>
       </c>
+      <c r="F78" t="n">
+        <v>0.1361637232608489</v>
+      </c>
+      <c r="G78" t="n">
+        <v>3.985562697683911e-05</v>
+      </c>
     </row>
     <row r="79">
       <c r="A79">
@@ -8777,6 +9249,12 @@
         <f>'Game'!E79/'Game'!G79</f>
         <v/>
       </c>
+      <c r="F79" t="n">
+        <v>0.1501149655463637</v>
+      </c>
+      <c r="G79" t="n">
+        <v>5.994075365997118e-06</v>
+      </c>
     </row>
     <row r="80">
       <c r="A80">
@@ -8799,6 +9277,12 @@
         <f>'Game'!E80/'Game'!G80</f>
         <v/>
       </c>
+      <c r="F80" t="n">
+        <v>0.06491135543024058</v>
+      </c>
+      <c r="G80" t="n">
+        <v>3.647615215831397e-06</v>
+      </c>
     </row>
     <row r="81">
       <c r="A81">
@@ -8821,6 +9305,12 @@
         <f>'Game'!E81/'Game'!G81</f>
         <v/>
       </c>
+      <c r="F81" t="n">
+        <v>0.1292069124664514</v>
+      </c>
+      <c r="G81" t="n">
+        <v>4.910732999991599e-06</v>
+      </c>
     </row>
     <row r="82">
       <c r="A82">
@@ -8843,6 +9333,12 @@
         <f>'Game'!E82/'Game'!G82</f>
         <v/>
       </c>
+      <c r="F82" t="n">
+        <v>0.08640350922668513</v>
+      </c>
+      <c r="G82" t="n">
+        <v>0.0008691371484514061</v>
+      </c>
     </row>
     <row r="83">
       <c r="A83">
@@ -8865,6 +9361,12 @@
         <f>'Game'!E83/'Game'!G83</f>
         <v/>
       </c>
+      <c r="F83" t="n">
+        <v>0.1113336671116673</v>
+      </c>
+      <c r="G83" t="n">
+        <v>4.776748461687954e-06</v>
+      </c>
     </row>
     <row r="84">
       <c r="A84">
@@ -8887,6 +9389,12 @@
         <f>'Game'!E84/'Game'!G84</f>
         <v/>
       </c>
+      <c r="F84" t="n">
+        <v>0.4036366043505568</v>
+      </c>
+      <c r="G84" t="n">
+        <v>9.873319144550946e-06</v>
+      </c>
     </row>
     <row r="85">
       <c r="A85">
@@ -8909,6 +9417,12 @@
         <f>'Game'!E85/'Game'!G85</f>
         <v/>
       </c>
+      <c r="F85" t="n">
+        <v>0.1044622513119414</v>
+      </c>
+      <c r="G85" t="n">
+        <v>5.444988929724946e-06</v>
+      </c>
     </row>
     <row r="86">
       <c r="A86">
@@ -8931,6 +9445,12 @@
         <f>'Game'!E86/'Game'!G86</f>
         <v/>
       </c>
+      <c r="F86" t="n">
+        <v>0.2465364099762438</v>
+      </c>
+      <c r="G86" t="n">
+        <v>2.602152625945831e-05</v>
+      </c>
     </row>
     <row r="87">
       <c r="A87">
@@ -8953,6 +9473,12 @@
         <f>'Game'!E87/'Game'!G87</f>
         <v/>
       </c>
+      <c r="F87" t="n">
+        <v>0.2665267223689748</v>
+      </c>
+      <c r="G87" t="n">
+        <v>2.719812161852009e-06</v>
+      </c>
     </row>
     <row r="88">
       <c r="A88">
@@ -8975,6 +9501,12 @@
         <f>'Game'!E88/'Game'!G88</f>
         <v/>
       </c>
+      <c r="F88" t="n">
+        <v>0.007340226177618909</v>
+      </c>
+      <c r="G88" t="n">
+        <v>8.389530498226924e-08</v>
+      </c>
     </row>
     <row r="89">
       <c r="A89">
@@ -8997,6 +9529,12 @@
         <f>'Game'!E89/'Game'!G89</f>
         <v/>
       </c>
+      <c r="F89" t="n">
+        <v>0.00751953062728887</v>
+      </c>
+      <c r="G89" t="n">
+        <v>3.543716678526202e-07</v>
+      </c>
     </row>
     <row r="90">
       <c r="A90">
@@ -9019,6 +9557,12 @@
         <f>'Game'!E90/'Game'!G90</f>
         <v/>
       </c>
+      <c r="F90" t="n">
+        <v>0.4444444444444444</v>
+      </c>
+      <c r="G90" t="n">
+        <v>0.0006376900316294255</v>
+      </c>
     </row>
     <row r="91">
       <c r="A91">
@@ -9041,6 +9585,12 @@
         <f>'Game'!E91/'Game'!G91</f>
         <v/>
       </c>
+      <c r="F91" t="n">
+        <v>0.00762761961061002</v>
+      </c>
+      <c r="G91" t="n">
+        <v>1.369712157729477e-07</v>
+      </c>
     </row>
     <row r="92">
       <c r="A92">
@@ -9063,6 +9613,12 @@
         <f>'Game'!E92/'Game'!G92</f>
         <v/>
       </c>
+      <c r="F92" t="n">
+        <v>0.3736228262623968</v>
+      </c>
+      <c r="G92" t="n">
+        <v>6.811451534380811e-06</v>
+      </c>
     </row>
     <row r="93">
       <c r="A93">
@@ -9085,6 +9641,12 @@
         <f>'Game'!E93/'Game'!G93</f>
         <v/>
       </c>
+      <c r="F93" t="n">
+        <v>0.1664613366079607</v>
+      </c>
+      <c r="G93" t="n">
+        <v>2.090389606762649e-06</v>
+      </c>
     </row>
     <row r="94">
       <c r="A94">
@@ -9107,6 +9669,12 @@
         <f>'Game'!E94/'Game'!G94</f>
         <v/>
       </c>
+      <c r="F94" t="n">
+        <v>0.04385844686275046</v>
+      </c>
+      <c r="G94" t="n">
+        <v>1.271510887154304e-05</v>
+      </c>
     </row>
     <row r="95">
       <c r="A95">
@@ -9129,6 +9697,12 @@
         <f>'Game'!E95/'Game'!G95</f>
         <v/>
       </c>
+      <c r="F95" t="n">
+        <v>0.1123058456540333</v>
+      </c>
+      <c r="G95" t="n">
+        <v>4.656164919498982e-05</v>
+      </c>
     </row>
     <row r="96">
       <c r="A96">
@@ -9151,6 +9725,12 @@
         <f>'Game'!E96/'Game'!G96</f>
         <v/>
       </c>
+      <c r="F96" t="n">
+        <v>0.1858975476478136</v>
+      </c>
+      <c r="G96" t="n">
+        <v>8.793238792432781e-07</v>
+      </c>
     </row>
     <row r="97">
       <c r="A97">
@@ -9173,6 +9753,12 @@
         <f>'Game'!E97/'Game'!G97</f>
         <v/>
       </c>
+      <c r="F97" t="n">
+        <v>0.2304737456984956</v>
+      </c>
+      <c r="G97" t="n">
+        <v>5.993194952475595e-06</v>
+      </c>
     </row>
     <row r="98">
       <c r="A98">
@@ -9195,6 +9781,12 @@
         <f>'Game'!E98/'Game'!G98</f>
         <v/>
       </c>
+      <c r="F98" t="n">
+        <v>0.1303288196118808</v>
+      </c>
+      <c r="G98" t="n">
+        <v>1.990456002323579e-06</v>
+      </c>
     </row>
     <row r="99">
       <c r="A99">
@@ -9217,6 +9809,12 @@
         <f>'Game'!E99/'Game'!G99</f>
         <v/>
       </c>
+      <c r="F99" t="n">
+        <v>0.1925357360766339</v>
+      </c>
+      <c r="G99" t="n">
+        <v>9.921465621919468e-05</v>
+      </c>
     </row>
     <row r="100">
       <c r="A100">
@@ -9239,6 +9837,12 @@
         <f>'Game'!E100/'Game'!G100</f>
         <v/>
       </c>
+      <c r="F100" t="n">
+        <v>0.11103707405762</v>
+      </c>
+      <c r="G100" t="n">
+        <v>4.596380350474002e-05</v>
+      </c>
     </row>
     <row r="101">
       <c r="A101">
@@ -9261,6 +9865,12 @@
         <f>'Game'!E101/'Game'!G101</f>
         <v/>
       </c>
+      <c r="F101" t="n">
+        <v>0.07597407885987827</v>
+      </c>
+      <c r="G101" t="n">
+        <v>0.0007639463758536718</v>
+      </c>
     </row>
     <row r="102">
       <c r="A102">
@@ -9283,6 +9893,12 @@
         <f>'Game'!E102/'Game'!G102</f>
         <v/>
       </c>
+      <c r="F102" t="n">
+        <v>0.232627867784659</v>
+      </c>
+      <c r="G102" t="n">
+        <v>0.001085631932777671</v>
+      </c>
     </row>
     <row r="103">
       <c r="A103">
@@ -9305,6 +9921,12 @@
         <f>'Game'!E103/'Game'!G103</f>
         <v/>
       </c>
+      <c r="F103" t="n">
+        <v>0.07473303119267043</v>
+      </c>
+      <c r="G103" t="n">
+        <v>0.0001894127515240339</v>
+      </c>
     </row>
     <row r="104">
       <c r="A104">
@@ -9327,6 +9949,12 @@
         <f>'Game'!E104/'Game'!G104</f>
         <v/>
       </c>
+      <c r="F104" t="n">
+        <v>0.09864018585389257</v>
+      </c>
+      <c r="G104" t="n">
+        <v>0.003958028668199546</v>
+      </c>
     </row>
     <row r="105">
       <c r="A105">
@@ -9349,6 +9977,12 @@
         <f>'Game'!E105/'Game'!G105</f>
         <v/>
       </c>
+      <c r="F105" t="n">
+        <v>0.04082865678496131</v>
+      </c>
+      <c r="G105" t="n">
+        <v>0.00041010761059659</v>
+      </c>
     </row>
     <row r="106">
       <c r="A106">
@@ -9371,6 +10005,12 @@
         <f>'Game'!E106/'Game'!G106</f>
         <v/>
       </c>
+      <c r="F106" t="n">
+        <v>0.006406148426512855</v>
+      </c>
+      <c r="G106" t="n">
+        <v>7.15799052039972e-06</v>
+      </c>
     </row>
     <row r="107">
       <c r="A107">
@@ -9393,6 +10033,12 @@
         <f>'Game'!E107/'Game'!G107</f>
         <v/>
       </c>
+      <c r="F107" t="n">
+        <v>0.3145555220379171</v>
+      </c>
+      <c r="G107" t="n">
+        <v>3.763784862057285e-05</v>
+      </c>
     </row>
     <row r="108">
       <c r="A108">
@@ -9415,6 +10061,12 @@
         <f>'Game'!E108/'Game'!G108</f>
         <v/>
       </c>
+      <c r="F108" t="n">
+        <v>0.1714611490468903</v>
+      </c>
+      <c r="G108" t="n">
+        <v>5.32958365927074e-06</v>
+      </c>
     </row>
     <row r="109">
       <c r="A109">
@@ -9437,6 +10089,12 @@
         <f>'Game'!E109/'Game'!G109</f>
         <v/>
       </c>
+      <c r="F109" t="n">
+        <v>0.2083124586890356</v>
+      </c>
+      <c r="G109" t="n">
+        <v>4.077711392636306e-05</v>
+      </c>
     </row>
     <row r="110">
       <c r="A110">
@@ -9459,6 +10117,12 @@
         <f>'Game'!E110/'Game'!G110</f>
         <v/>
       </c>
+      <c r="F110" t="n">
+        <v>0.1608997772986183</v>
+      </c>
+      <c r="G110" t="n">
+        <v>0.0001834569897654299</v>
+      </c>
     </row>
     <row r="111">
       <c r="A111">
@@ -9481,6 +10145,12 @@
         <f>'Game'!E111/'Game'!G111</f>
         <v/>
       </c>
+      <c r="F111" t="n">
+        <v>0.3142029801524261</v>
+      </c>
+      <c r="G111" t="n">
+        <v>6.51185743102137e-06</v>
+      </c>
     </row>
     <row r="112">
       <c r="A112">
@@ -9503,6 +10173,12 @@
         <f>'Game'!E112/'Game'!G112</f>
         <v/>
       </c>
+      <c r="F112" t="n">
+        <v>0.04349334171305051</v>
+      </c>
+      <c r="G112" t="n">
+        <v>0.0004441478523785783</v>
+      </c>
     </row>
     <row r="113">
       <c r="A113">
@@ -9525,6 +10201,12 @@
         <f>'Game'!E113/'Game'!G113</f>
         <v/>
       </c>
+      <c r="F113" t="n">
+        <v>0.1022036747535665</v>
+      </c>
+      <c r="G113" t="n">
+        <v>0.0002589747975050161</v>
+      </c>
     </row>
     <row r="114">
       <c r="A114">
@@ -9547,6 +10229,12 @@
         <f>'Game'!E114/'Game'!G114</f>
         <v/>
       </c>
+      <c r="F114" t="n">
+        <v>0.04925129171362776</v>
+      </c>
+      <c r="G114" t="n">
+        <v>1.430897462780698e-05</v>
+      </c>
     </row>
     <row r="115">
       <c r="A115">
@@ -9569,6 +10257,12 @@
         <f>'Game'!E115/'Game'!G115</f>
         <v/>
       </c>
+      <c r="F115" t="n">
+        <v>0.07073336351290177</v>
+      </c>
+      <c r="G115" t="n">
+        <v>1.862721521828582e-05</v>
+      </c>
     </row>
     <row r="116">
       <c r="A116">
@@ -9591,6 +10285,12 @@
         <f>'Game'!E116/'Game'!G116</f>
         <v/>
       </c>
+      <c r="F116" t="n">
+        <v>0.1869169709207661</v>
+      </c>
+      <c r="G116" t="n">
+        <v>0.0002144929267096545</v>
+      </c>
     </row>
     <row r="117">
       <c r="A117">
@@ -9613,6 +10313,12 @@
         <f>'Game'!E117/'Game'!G117</f>
         <v/>
       </c>
+      <c r="F117" t="n">
+        <v>0.01485760118442419</v>
+      </c>
+      <c r="G117" t="n">
+        <v>0.0005950291178242594</v>
+      </c>
     </row>
     <row r="118">
       <c r="A118">
@@ -9635,6 +10341,12 @@
         <f>'Game'!E118/'Game'!G118</f>
         <v/>
       </c>
+      <c r="F118" t="n">
+        <v>0.1542706116336086</v>
+      </c>
+      <c r="G118" t="n">
+        <v>0.000693798236430794</v>
+      </c>
     </row>
     <row r="119">
       <c r="A119">
@@ -9657,6 +10369,12 @@
         <f>'Game'!E119/'Game'!G119</f>
         <v/>
       </c>
+      <c r="F119" t="n">
+        <v>0.3173973417972625</v>
+      </c>
+      <c r="G119" t="n">
+        <v>0.01306122448979592</v>
+      </c>
     </row>
     <row r="120">
       <c r="A120">
@@ -9679,6 +10397,12 @@
         <f>'Game'!E120/'Game'!G120</f>
         <v/>
       </c>
+      <c r="F120" t="n">
+        <v>0.2402921953094964</v>
+      </c>
+      <c r="G120" t="n">
+        <v>0.000394066831271666</v>
+      </c>
     </row>
     <row r="121">
       <c r="A121">
@@ -9701,6 +10425,12 @@
         <f>'Game'!E121/'Game'!G121</f>
         <v/>
       </c>
+      <c r="F121" t="n">
+        <v>0.167279327202546</v>
+      </c>
+      <c r="G121" t="n">
+        <v>2.878115271970381e-05</v>
+      </c>
     </row>
     <row r="122">
       <c r="A122">
@@ -9723,6 +10453,12 @@
         <f>'Game'!E122/'Game'!G122</f>
         <v/>
       </c>
+      <c r="F122" t="n">
+        <v>0.3472452513343767</v>
+      </c>
+      <c r="G122" t="n">
+        <v>1.877358477641487e-05</v>
+      </c>
     </row>
     <row r="123">
       <c r="A123">
@@ -9745,6 +10481,12 @@
         <f>'Game'!E123/'Game'!G123</f>
         <v/>
       </c>
+      <c r="F123" t="n">
+        <v>0.1481568400160958</v>
+      </c>
+      <c r="G123" t="n">
+        <v>2.259389284401309e-06</v>
+      </c>
     </row>
     <row r="124">
       <c r="A124">
@@ -9767,6 +10509,12 @@
         <f>'Game'!E124/'Game'!G124</f>
         <v/>
       </c>
+      <c r="F124" t="n">
+        <v>0.2181557505528612</v>
+      </c>
+      <c r="G124" t="n">
+        <v>2.071955369988507e-06</v>
+      </c>
     </row>
     <row r="125">
       <c r="A125">
@@ -9789,6 +10537,12 @@
         <f>'Game'!E125/'Game'!G125</f>
         <v/>
       </c>
+      <c r="F125" t="n">
+        <v>0.1966558669819716</v>
+      </c>
+      <c r="G125" t="n">
+        <v>1.616682114904949e-06</v>
+      </c>
     </row>
     <row r="126">
       <c r="A126">
@@ -9811,6 +10565,12 @@
         <f>'Game'!E126/'Game'!G126</f>
         <v/>
       </c>
+      <c r="F126" t="n">
+        <v>0.1224608094059934</v>
+      </c>
+      <c r="G126" t="n">
+        <v>7.780706438447681e-07</v>
+      </c>
     </row>
     <row r="127">
       <c r="A127">
@@ -9833,6 +10593,12 @@
         <f>'Game'!E127/'Game'!G127</f>
         <v/>
       </c>
+      <c r="F127" t="n">
+        <v>0.2695798544053123</v>
+      </c>
+      <c r="G127" t="n">
+        <v>8.28400528500981e-06</v>
+      </c>
     </row>
     <row r="128">
       <c r="A128">
@@ -9855,6 +10621,12 @@
         <f>'Game'!E128/'Game'!G128</f>
         <v/>
       </c>
+      <c r="F128" t="n">
+        <v>0.135662661226594</v>
+      </c>
+      <c r="G128" t="n">
+        <v>4.329447394529899e-06</v>
+      </c>
     </row>
     <row r="129">
       <c r="A129">
@@ -9877,6 +10649,12 @@
         <f>'Game'!E129/'Game'!G129</f>
         <v/>
       </c>
+      <c r="F129" t="n">
+        <v>0.080364816082607</v>
+      </c>
+      <c r="G129" t="n">
+        <v>1.908571413302857e-05</v>
+      </c>
     </row>
     <row r="130">
       <c r="A130">
@@ -9899,6 +10677,12 @@
         <f>'Game'!E130/'Game'!G130</f>
         <v/>
       </c>
+      <c r="F130" t="n">
+        <v>0.2381859188772107</v>
+      </c>
+      <c r="G130" t="n">
+        <v>2.632316785590244e-06</v>
+      </c>
     </row>
     <row r="131">
       <c r="A131">
@@ -9921,6 +10705,12 @@
         <f>'Game'!E131/'Game'!G131</f>
         <v/>
       </c>
+      <c r="F131" t="n">
+        <v>0.1734665255574304</v>
+      </c>
+      <c r="G131" t="n">
+        <v>5.132110364161186e-06</v>
+      </c>
     </row>
     <row r="132">
       <c r="A132">
@@ -9943,6 +10733,12 @@
         <f>'Game'!E132/'Game'!G132</f>
         <v/>
       </c>
+      <c r="F132" t="n">
+        <v>0.2724011837465841</v>
+      </c>
+      <c r="G132" t="n">
+        <v>3.006560690645763e-06</v>
+      </c>
     </row>
     <row r="133">
       <c r="A133">
@@ -9965,6 +10761,12 @@
         <f>'Game'!E133/'Game'!G133</f>
         <v/>
       </c>
+      <c r="F133" t="n">
+        <v>0.1832543629198724</v>
+      </c>
+      <c r="G133" t="n">
+        <v>2.517008691106858e-06</v>
+      </c>
     </row>
     <row r="134">
       <c r="A134">
@@ -9987,6 +10789,12 @@
         <f>'Game'!E134/'Game'!G134</f>
         <v/>
       </c>
+      <c r="F134" t="n">
+        <v>0.1872406366106749</v>
+      </c>
+      <c r="G134" t="n">
+        <v>1.47026238265035e-06</v>
+      </c>
     </row>
     <row r="135">
       <c r="A135">
@@ -10009,6 +10817,12 @@
         <f>'Game'!E135/'Game'!G135</f>
         <v/>
       </c>
+      <c r="F135" t="n">
+        <v>0.4100122515007787</v>
+      </c>
+      <c r="G135" t="n">
+        <v>2.664934423034083e-06</v>
+      </c>
     </row>
     <row r="136">
       <c r="A136">
@@ -10031,6 +10845,12 @@
         <f>'Game'!E136/'Game'!G136</f>
         <v/>
       </c>
+      <c r="F136" t="n">
+        <v>0.332968289099051</v>
+      </c>
+      <c r="G136" t="n">
+        <v>7.569333046990511e-05</v>
+      </c>
     </row>
     <row r="137">
       <c r="A137">
@@ -10053,6 +10873,12 @@
         <f>'Game'!E137/'Game'!G137</f>
         <v/>
       </c>
+      <c r="F137" t="n">
+        <v>0.1481568400160958</v>
+      </c>
+      <c r="G137" t="n">
+        <v>1.231828982718671e-06</v>
+      </c>
     </row>
     <row r="138">
       <c r="A138">
@@ -10075,6 +10901,12 @@
         <f>'Game'!E138/'Game'!G138</f>
         <v/>
       </c>
+      <c r="F138" t="n">
+        <v>0.1398547412715258</v>
+      </c>
+      <c r="G138" t="n">
+        <v>2.143644768856784e-05</v>
+      </c>
     </row>
     <row r="139">
       <c r="A139">
@@ -10097,6 +10929,12 @@
         <f>'Game'!E139/'Game'!G139</f>
         <v/>
       </c>
+      <c r="F139" t="n">
+        <v>0.3089851968282052</v>
+      </c>
+      <c r="G139" t="n">
+        <v>3.017300977507455e-05</v>
+      </c>
     </row>
     <row r="140">
       <c r="A140">
@@ -10119,6 +10957,12 @@
         <f>'Game'!E140/'Game'!G140</f>
         <v/>
       </c>
+      <c r="F140" t="n">
+        <v>0.05389690554150647</v>
+      </c>
+      <c r="G140" t="n">
+        <v>1.527030779133317e-07</v>
+      </c>
     </row>
     <row r="141">
       <c r="A141">
@@ -10141,6 +10985,12 @@
         <f>'Game'!E141/'Game'!G141</f>
         <v/>
       </c>
+      <c r="F141" t="n">
+        <v>0.1969917150413432</v>
+      </c>
+      <c r="G141" t="n">
+        <v>8.134704351873754e-07</v>
+      </c>
     </row>
     <row r="142">
       <c r="A142">
@@ -10163,6 +11013,12 @@
         <f>'Game'!E142/'Game'!G142</f>
         <v/>
       </c>
+      <c r="F142" t="n">
+        <v>0.2896733758882834</v>
+      </c>
+      <c r="G142" t="n">
+        <v>7.942986362264148e-06</v>
+      </c>
     </row>
     <row r="143">
       <c r="A143">
@@ -10185,6 +11041,12 @@
         <f>'Game'!E143/'Game'!G143</f>
         <v/>
       </c>
+      <c r="F143" t="n">
+        <v>0.3431886827354471</v>
+      </c>
+      <c r="G143" t="n">
+        <v>8.681642863498871e-06</v>
+      </c>
     </row>
     <row r="144">
       <c r="A144">
@@ -10207,6 +11069,12 @@
         <f>'Game'!E144/'Game'!G144</f>
         <v/>
       </c>
+      <c r="F144" t="n">
+        <v>0.3930778982124782</v>
+      </c>
+      <c r="G144" t="n">
+        <v>4.935200335939481e-06</v>
+      </c>
     </row>
     <row r="145">
       <c r="A145">
@@ -10229,6 +11097,12 @@
         <f>'Game'!E145/'Game'!G145</f>
         <v/>
       </c>
+      <c r="F145" t="n">
+        <v>0.3472452513343767</v>
+      </c>
+      <c r="G145" t="n">
+        <v>3.230140831717657e-05</v>
+      </c>
     </row>
     <row r="146">
       <c r="A146">
@@ -10251,6 +11125,12 @@
         <f>'Game'!E146/'Game'!G146</f>
         <v/>
       </c>
+      <c r="F146" t="n">
+        <v>0.3357857111530196</v>
+      </c>
+      <c r="G146" t="n">
+        <v>1.431186183010548e-05</v>
+      </c>
     </row>
     <row r="147">
       <c r="A147">
@@ -10273,6 +11153,12 @@
         <f>'Game'!E147/'Game'!G147</f>
         <v/>
       </c>
+      <c r="F147" t="n">
+        <v>0.1843575903061829</v>
+      </c>
+      <c r="G147" t="n">
+        <v>2.576256213807212e-06</v>
+      </c>
     </row>
     <row r="148">
       <c r="A148">
@@ -10295,6 +11181,12 @@
         <f>'Game'!E148/'Game'!G148</f>
         <v/>
       </c>
+      <c r="F148" t="n">
+        <v>0.0887883725588525</v>
+      </c>
+      <c r="G148" t="n">
+        <v>1.674772009400889e-06</v>
+      </c>
     </row>
     <row r="149">
       <c r="A149">
@@ -10317,6 +11209,12 @@
         <f>'Game'!E149/'Game'!G149</f>
         <v/>
       </c>
+      <c r="F149" t="n">
+        <v>0.2780403179626745</v>
+      </c>
+      <c r="G149" t="n">
+        <v>8.26313711977901e-05</v>
+      </c>
     </row>
     <row r="150">
       <c r="A150">
@@ -10339,6 +11237,12 @@
         <f>'Game'!E150/'Game'!G150</f>
         <v/>
       </c>
+      <c r="F150" t="n">
+        <v>0.3646526173306261</v>
+      </c>
+      <c r="G150" t="n">
+        <v>6.215301400827362e-06</v>
+      </c>
     </row>
     <row r="151">
       <c r="A151">
@@ -10361,6 +11265,12 @@
         <f>'Game'!E151/'Game'!G151</f>
         <v/>
       </c>
+      <c r="F151" t="n">
+        <v>0.25</v>
+      </c>
+      <c r="G151" t="n">
+        <v>5.836072883212594e-05</v>
+      </c>
     </row>
     <row r="152">
       <c r="A152">
@@ -10383,6 +11293,12 @@
         <f>'Game'!E152/'Game'!G152</f>
         <v/>
       </c>
+      <c r="F152" t="n">
+        <v>0.07255495470983687</v>
+      </c>
+      <c r="G152" t="n">
+        <v>1.500132345660261e-05</v>
+      </c>
     </row>
     <row r="153">
       <c r="A153">
@@ -10405,6 +11321,12 @@
         <f>'Game'!E153/'Game'!G153</f>
         <v/>
       </c>
+      <c r="F153" t="n">
+        <v>0.2155304333282468</v>
+      </c>
+      <c r="G153" t="n">
+        <v>3.291884712551126e-06</v>
+      </c>
     </row>
     <row r="154">
       <c r="A154">
@@ -10427,6 +11349,12 @@
         <f>'Game'!E154/'Game'!G154</f>
         <v/>
       </c>
+      <c r="F154" t="n">
+        <v>0.11490950876185</v>
+      </c>
+      <c r="G154" t="n">
+        <v>4.092070669344348e-05</v>
+      </c>
     </row>
     <row r="155">
       <c r="A155">
@@ -10449,6 +11377,12 @@
         <f>'Game'!E155/'Game'!G155</f>
         <v/>
       </c>
+      <c r="F155" t="n">
+        <v>0.1809234004697857</v>
+      </c>
+      <c r="G155" t="n">
+        <v>4.381164078320804e-06</v>
+      </c>
     </row>
     <row r="156">
       <c r="A156">
@@ -10471,6 +11405,12 @@
         <f>'Game'!E156/'Game'!G156</f>
         <v/>
       </c>
+      <c r="F156" t="n">
+        <v>0.5193362714203466</v>
+      </c>
+      <c r="G156" t="n">
+        <v>1.754137491349347e-05</v>
+      </c>
     </row>
     <row r="157">
       <c r="A157">
@@ -10493,6 +11433,12 @@
         <f>'Game'!E157/'Game'!G157</f>
         <v/>
       </c>
+      <c r="F157" t="n">
+        <v>0.3695457359041399</v>
+      </c>
+      <c r="G157" t="n">
+        <v>0.0001174124734498751</v>
+      </c>
     </row>
     <row r="158">
       <c r="A158">
@@ -10515,6 +11461,12 @@
         <f>'Game'!E158/'Game'!G158</f>
         <v/>
       </c>
+      <c r="F158" t="n">
+        <v>0.2668021310019807</v>
+      </c>
+      <c r="G158" t="n">
+        <v>2.579028951400399e-06</v>
+      </c>
     </row>
     <row r="159">
       <c r="A159">
@@ -10537,6 +11489,12 @@
         <f>'Game'!E159/'Game'!G159</f>
         <v/>
       </c>
+      <c r="F159" t="n">
+        <v>0.1263748158245028</v>
+      </c>
+      <c r="G159" t="n">
+        <v>1.42920349253993e-06</v>
+      </c>
     </row>
     <row r="160">
       <c r="A160">
@@ -10559,6 +11517,12 @@
         <f>'Game'!E160/'Game'!G160</f>
         <v/>
       </c>
+      <c r="F160" t="n">
+        <v>0.2755561066677689</v>
+      </c>
+      <c r="G160" t="n">
+        <v>2.877027278283263e-06</v>
+      </c>
     </row>
     <row r="161">
       <c r="A161">
@@ -10581,6 +11545,12 @@
         <f>'Game'!E161/'Game'!G161</f>
         <v/>
       </c>
+      <c r="F161" t="n">
+        <v>0.1570961345082239</v>
+      </c>
+      <c r="G161" t="n">
+        <v>3.115579542864947e-06</v>
+      </c>
     </row>
     <row r="162">
       <c r="A162">
@@ -10603,6 +11573,12 @@
         <f>'Game'!E162/'Game'!G162</f>
         <v/>
       </c>
+      <c r="F162" t="n">
+        <v>0.195786670843449</v>
+      </c>
+      <c r="G162" t="n">
+        <v>0.0005510370517313583</v>
+      </c>
     </row>
     <row r="163">
       <c r="A163">
@@ -10625,6 +11601,12 @@
         <f>'Game'!E163/'Game'!G163</f>
         <v/>
       </c>
+      <c r="F163" t="n">
+        <v>0.3843538761511879</v>
+      </c>
+      <c r="G163" t="n">
+        <v>8.954453605133045e-06</v>
+      </c>
     </row>
     <row r="164">
       <c r="A164">
@@ -10647,6 +11629,12 @@
         <f>'Game'!E164/'Game'!G164</f>
         <v/>
       </c>
+      <c r="F164" t="n">
+        <v>0.1631168099049747</v>
+      </c>
+      <c r="G164" t="n">
+        <v>8.355034030320964e-06</v>
+      </c>
     </row>
     <row r="165">
       <c r="A165">
@@ -10669,6 +11657,12 @@
         <f>'Game'!E165/'Game'!G165</f>
         <v/>
       </c>
+      <c r="F165" t="n">
+        <v>0.01608409407747467</v>
+      </c>
+      <c r="G165" t="n">
+        <v>5.559373633298179e-07</v>
+      </c>
     </row>
     <row r="166">
       <c r="A166">
@@ -10691,6 +11685,12 @@
         <f>'Game'!E166/'Game'!G166</f>
         <v/>
       </c>
+      <c r="F166" t="n">
+        <v>0.1514027464458206</v>
+      </c>
+      <c r="G166" t="n">
+        <v>2.739293444180485e-06</v>
+      </c>
     </row>
     <row r="167">
       <c r="A167">
@@ -10713,6 +11713,12 @@
         <f>'Game'!E167/'Game'!G167</f>
         <v/>
       </c>
+      <c r="F167" t="n">
+        <v>0.2051170972484772</v>
+      </c>
+      <c r="G167" t="n">
+        <v>2.808069594325763e-06</v>
+      </c>
     </row>
     <row r="168">
       <c r="A168">
@@ -10735,6 +11741,12 @@
         <f>'Game'!E168/'Game'!G168</f>
         <v/>
       </c>
+      <c r="F168" t="n">
+        <v>0.1077097682742816</v>
+      </c>
+      <c r="G168" t="n">
+        <v>2.211563326277845e-06</v>
+      </c>
     </row>
     <row r="169">
       <c r="A169">
@@ -10757,6 +11769,12 @@
         <f>'Game'!E169/'Game'!G169</f>
         <v/>
       </c>
+      <c r="F169" t="n">
+        <v>0.1747743313833179</v>
+      </c>
+      <c r="G169" t="n">
+        <v>3.799839646766906e-06</v>
+      </c>
     </row>
     <row r="170">
       <c r="A170">
@@ -10779,6 +11797,12 @@
         <f>'Game'!E170/'Game'!G170</f>
         <v/>
       </c>
+      <c r="F170" t="n">
+        <v>0.05063512651895252</v>
+      </c>
+      <c r="G170" t="n">
+        <v>9.537488265780212e-07</v>
+      </c>
     </row>
     <row r="171">
       <c r="A171">
@@ -10801,6 +11825,12 @@
         <f>'Game'!E171/'Game'!G171</f>
         <v/>
       </c>
+      <c r="F171" t="n">
+        <v>0.1014239928597509</v>
+      </c>
+      <c r="G171" t="n">
+        <v>1.905071287976202e-06</v>
+      </c>
     </row>
     <row r="172">
       <c r="A172">
@@ -10823,6 +11853,12 @@
         <f>'Game'!E172/'Game'!G172</f>
         <v/>
       </c>
+      <c r="F172" t="n">
+        <v>0.02380761863318509</v>
+      </c>
+      <c r="G172" t="n">
+        <v>3.152558403990159e-08</v>
+      </c>
     </row>
     <row r="173">
       <c r="A173">
@@ -10845,6 +11881,12 @@
         <f>'Game'!E173/'Game'!G173</f>
         <v/>
       </c>
+      <c r="F173" t="n">
+        <v>0.09193448308102917</v>
+      </c>
+      <c r="G173" t="n">
+        <v>9.833268206174894e-07</v>
+      </c>
     </row>
     <row r="174">
       <c r="A174">
@@ -10867,6 +11909,12 @@
         <f>'Game'!E174/'Game'!G174</f>
         <v/>
       </c>
+      <c r="F174" t="n">
+        <v>0.04111060462846208</v>
+      </c>
+      <c r="G174" t="n">
+        <v>1.17286622282737e-06</v>
+      </c>
     </row>
     <row r="175">
       <c r="A175">
@@ -10889,6 +11937,12 @@
         <f>'Game'!E175/'Game'!G175</f>
         <v/>
       </c>
+      <c r="F175" t="n">
+        <v>0.1573454934126522</v>
+      </c>
+      <c r="G175" t="n">
+        <v>2.940119411185813e-06</v>
+      </c>
     </row>
     <row r="176">
       <c r="A176">
@@ -10911,6 +11965,12 @@
         <f>'Game'!E176/'Game'!G176</f>
         <v/>
       </c>
+      <c r="F176" t="n">
+        <v>0.1659193383136788</v>
+      </c>
+      <c r="G176" t="n">
+        <v>0.0004585283989563893</v>
+      </c>
     </row>
     <row r="177">
       <c r="A177">
@@ -10933,6 +11993,12 @@
         <f>'Game'!E177/'Game'!G177</f>
         <v/>
       </c>
+      <c r="F177" t="n">
+        <v>0.1959600484491624</v>
+      </c>
+      <c r="G177" t="n">
+        <v>1.922385095128888e-06</v>
+      </c>
     </row>
     <row r="178">
       <c r="A178">
@@ -10955,6 +12021,12 @@
         <f>'Game'!E178/'Game'!G178</f>
         <v/>
       </c>
+      <c r="F178" t="n">
+        <v>0.1665056462472193</v>
+      </c>
+      <c r="G178" t="n">
+        <v>1.525010340047859e-06</v>
+      </c>
     </row>
     <row r="179">
       <c r="A179">
@@ -10977,6 +12049,12 @@
         <f>'Game'!E179/'Game'!G179</f>
         <v/>
       </c>
+      <c r="F179" t="n">
+        <v>0.4036366043505568</v>
+      </c>
+      <c r="G179" t="n">
+        <v>4.438484731210398e-06</v>
+      </c>
     </row>
     <row r="180">
       <c r="A180">
@@ -10999,6 +12077,12 @@
         <f>'Game'!E180/'Game'!G180</f>
         <v/>
       </c>
+      <c r="F180" t="n">
+        <v>0.1694066452290914</v>
+      </c>
+      <c r="G180" t="n">
+        <v>2.112137224548412e-06</v>
+      </c>
     </row>
     <row r="181">
       <c r="A181">
@@ -11021,6 +12105,12 @@
         <f>'Game'!E181/'Game'!G181</f>
         <v/>
       </c>
+      <c r="F181" t="n">
+        <v>0.3642126142125232</v>
+      </c>
+      <c r="G181" t="n">
+        <v>4.589508902937561e-06</v>
+      </c>
     </row>
     <row r="182">
       <c r="A182">
@@ -11043,6 +12133,12 @@
         <f>'Game'!E182/'Game'!G182</f>
         <v/>
       </c>
+      <c r="F182" t="n">
+        <v>0.1564753244672328</v>
+      </c>
+      <c r="G182" t="n">
+        <v>1.711428040201308e-06</v>
+      </c>
     </row>
     <row r="183">
       <c r="A183">
@@ -11065,6 +12161,12 @@
         <f>'Game'!E183/'Game'!G183</f>
         <v/>
       </c>
+      <c r="F183" t="n">
+        <v>0.2912387519953495</v>
+      </c>
+      <c r="G183" t="n">
+        <v>4.417984104814206e-06</v>
+      </c>
     </row>
     <row r="184">
       <c r="A184">
@@ -11087,6 +12189,12 @@
         <f>'Game'!E184/'Game'!G184</f>
         <v/>
       </c>
+      <c r="F184" t="n">
+        <v>0.378698224852071</v>
+      </c>
+      <c r="G184" t="n">
+        <v>7.440722000042265e-06</v>
+      </c>
     </row>
     <row r="185">
       <c r="A185">
@@ -11109,6 +12217,12 @@
         <f>'Game'!E185/'Game'!G185</f>
         <v/>
       </c>
+      <c r="F185" t="n">
+        <v>0.2260392152923064</v>
+      </c>
+      <c r="G185" t="n">
+        <v>1.813988972773631e-05</v>
+      </c>
     </row>
     <row r="186">
       <c r="A186">
@@ -11131,6 +12245,12 @@
         <f>'Game'!E186/'Game'!G186</f>
         <v/>
       </c>
+      <c r="F186" t="n">
+        <v>0.2462917695447912</v>
+      </c>
+      <c r="G186" t="n">
+        <v>5.289256198347107e-05</v>
+      </c>
     </row>
     <row r="187">
       <c r="A187">
@@ -11153,6 +12273,12 @@
         <f>'Game'!E187/'Game'!G187</f>
         <v/>
       </c>
+      <c r="F187" t="n">
+        <v>0.3399943900925634</v>
+      </c>
+      <c r="G187" t="n">
+        <v>5.769042312369323e-06</v>
+      </c>
     </row>
     <row r="188">
       <c r="A188">
@@ -11175,6 +12301,12 @@
         <f>'Game'!E188/'Game'!G188</f>
         <v/>
       </c>
+      <c r="F188" t="n">
+        <v>0.297693839652286</v>
+      </c>
+      <c r="G188" t="n">
+        <v>9.317774885540456e-06</v>
+      </c>
     </row>
     <row r="189">
       <c r="A189">
@@ -11197,6 +12329,12 @@
         <f>'Game'!E189/'Game'!G189</f>
         <v/>
       </c>
+      <c r="F189" t="n">
+        <v>0.06181813056533174</v>
+      </c>
+      <c r="G189" t="n">
+        <v>5.150118479570022e-07</v>
+      </c>
     </row>
     <row r="190">
       <c r="A190">
@@ -11219,6 +12357,12 @@
         <f>'Game'!E190/'Game'!G190</f>
         <v/>
       </c>
+      <c r="F190" t="n">
+        <v>0.0545049887204954</v>
+      </c>
+      <c r="G190" t="n">
+        <v>6.929038027792527e-07</v>
+      </c>
     </row>
     <row r="191">
       <c r="A191">
@@ -11241,6 +12385,12 @@
         <f>'Game'!E191/'Game'!G191</f>
         <v/>
       </c>
+      <c r="F191" t="n">
+        <v>0.418494513671924</v>
+      </c>
+      <c r="G191" t="n">
+        <v>1.155809097196027e-05</v>
+      </c>
     </row>
     <row r="192">
       <c r="A192">
@@ -11263,6 +12413,12 @@
         <f>'Game'!E192/'Game'!G192</f>
         <v/>
       </c>
+      <c r="F192" t="n">
+        <v>0.01437698761853826</v>
+      </c>
+      <c r="G192" t="n">
+        <v>3.972510923570813e-07</v>
+      </c>
     </row>
     <row r="193">
       <c r="A193">
@@ -11285,6 +12441,12 @@
         <f>'Game'!E193/'Game'!G193</f>
         <v/>
       </c>
+      <c r="F193" t="n">
+        <v>0.1333443164601991</v>
+      </c>
+      <c r="G193" t="n">
+        <v>2.928643922497277e-07</v>
+      </c>
     </row>
     <row r="194">
       <c r="A194">
@@ -11307,6 +12469,12 @@
         <f>'Game'!E194/'Game'!G194</f>
         <v/>
       </c>
+      <c r="F194" t="n">
+        <v>0.04548199797505049</v>
+      </c>
+      <c r="G194" t="n">
+        <v>6.198060101398775e-07</v>
+      </c>
     </row>
     <row r="195">
       <c r="A195">
@@ -11329,6 +12497,12 @@
         <f>'Game'!E195/'Game'!G195</f>
         <v/>
       </c>
+      <c r="F195" t="n">
+        <v>0.4232834954274931</v>
+      </c>
+      <c r="G195" t="n">
+        <v>0.000381028593640082</v>
+      </c>
     </row>
     <row r="196">
       <c r="A196">
@@ -11351,6 +12525,12 @@
         <f>'Game'!E196/'Game'!G196</f>
         <v/>
       </c>
+      <c r="F196" t="n">
+        <v>0.2826327009991914</v>
+      </c>
+      <c r="G196" t="n">
+        <v>1.344713373672045e-05</v>
+      </c>
     </row>
     <row r="197">
       <c r="A197">
@@ -11373,6 +12553,12 @@
         <f>'Game'!E197/'Game'!G197</f>
         <v/>
       </c>
+      <c r="F197" t="n">
+        <v>0.4559213006887602</v>
+      </c>
+      <c r="G197" t="n">
+        <v>6.67349988564958e-06</v>
+      </c>
     </row>
     <row r="198">
       <c r="A198">
@@ -11395,6 +12581,12 @@
         <f>'Game'!E198/'Game'!G198</f>
         <v/>
       </c>
+      <c r="F198" t="n">
+        <v>0.2193836416587598</v>
+      </c>
+      <c r="G198" t="n">
+        <v>2.135817009321174e-06</v>
+      </c>
     </row>
     <row r="199">
       <c r="A199">
@@ -11417,6 +12609,12 @@
         <f>'Game'!E199/'Game'!G199</f>
         <v/>
       </c>
+      <c r="F199" t="n">
+        <v>0.3624605416392858</v>
+      </c>
+      <c r="G199" t="n">
+        <v>1.518159714121416e-05</v>
+      </c>
     </row>
     <row r="200">
       <c r="A200">
@@ -11439,6 +12637,12 @@
         <f>'Game'!E200/'Game'!G200</f>
         <v/>
       </c>
+      <c r="F200" t="n">
+        <v>0.1803093206395572</v>
+      </c>
+      <c r="G200" t="n">
+        <v>4.78921468852145e-05</v>
+      </c>
     </row>
     <row r="201">
       <c r="A201">
@@ -11461,6 +12665,12 @@
         <f>'Game'!E201/'Game'!G201</f>
         <v/>
       </c>
+      <c r="F201" t="n">
+        <v>0.3138510306083218</v>
+      </c>
+      <c r="G201" t="n">
+        <v>0.0001024439017194185</v>
+      </c>
     </row>
     <row r="202">
       <c r="A202">
@@ -11483,6 +12693,12 @@
         <f>'Game'!E202/'Game'!G202</f>
         <v/>
       </c>
+      <c r="F202" t="n">
+        <v>0.2291517192909771</v>
+      </c>
+      <c r="G202" t="n">
+        <v>2.524572950377944e-06</v>
+      </c>
     </row>
     <row r="203">
       <c r="A203">
@@ -11505,6 +12721,12 @@
         <f>'Game'!E203/'Game'!G203</f>
         <v/>
       </c>
+      <c r="F203" t="n">
+        <v>0.08305027032862991</v>
+      </c>
+      <c r="G203" t="n">
+        <v>3.446003579191618e-05</v>
+      </c>
     </row>
     <row r="204">
       <c r="A204">
@@ -11527,6 +12749,12 @@
         <f>'Game'!E204/'Game'!G204</f>
         <v/>
       </c>
+      <c r="F204" t="n">
+        <v>0.1849924846803098</v>
+      </c>
+      <c r="G204" t="n">
+        <v>1.428844753509051e-06</v>
+      </c>
     </row>
     <row r="205">
       <c r="A205">
@@ -11549,6 +12777,12 @@
         <f>'Game'!E205/'Game'!G205</f>
         <v/>
       </c>
+      <c r="F205" t="n">
+        <v>0.05690592040090903</v>
+      </c>
+      <c r="G205" t="n">
+        <v>1.654068881091741e-05</v>
+      </c>
     </row>
     <row r="206">
       <c r="A206">
@@ -11571,6 +12805,12 @@
         <f>'Game'!E206/'Game'!G206</f>
         <v/>
       </c>
+      <c r="F206" t="n">
+        <v>0.4178490052477657</v>
+      </c>
+      <c r="G206" t="n">
+        <v>8.650107178287983e-05</v>
+      </c>
     </row>
     <row r="207">
       <c r="A207">
@@ -11593,6 +12833,12 @@
         <f>'Game'!E207/'Game'!G207</f>
         <v/>
       </c>
+      <c r="F207" t="n">
+        <v>0.4743148995590769</v>
+      </c>
+      <c r="G207" t="n">
+        <v>0.0002036159587998582</v>
+      </c>
     </row>
     <row r="208">
       <c r="A208">
@@ -11615,6 +12861,12 @@
         <f>'Game'!E208/'Game'!G208</f>
         <v/>
       </c>
+      <c r="F208" t="n">
+        <v>0.1890359168241966</v>
+      </c>
+      <c r="G208" t="n">
+        <v>0.0004340277777777778</v>
+      </c>
     </row>
     <row r="209">
       <c r="A209">
@@ -11637,6 +12889,12 @@
         <f>'Game'!E209/'Game'!G209</f>
         <v/>
       </c>
+      <c r="F209" t="n">
+        <v>0.340788769237952</v>
+      </c>
+      <c r="G209" t="n">
+        <v>4.030897857538448e-06</v>
+      </c>
     </row>
     <row r="210">
       <c r="A210">
@@ -11659,6 +12917,12 @@
         <f>'Game'!E210/'Game'!G210</f>
         <v/>
       </c>
+      <c r="F210" t="n">
+        <v>0.176541204717181</v>
+      </c>
+      <c r="G210" t="n">
+        <v>6.037302074598112e-05</v>
+      </c>
     </row>
     <row r="211">
       <c r="A211">
@@ -11681,6 +12945,12 @@
         <f>'Game'!E211/'Game'!G211</f>
         <v/>
       </c>
+      <c r="F211" t="n">
+        <v>0.1363649256320242</v>
+      </c>
+      <c r="G211" t="n">
+        <v>2.290201426330119e-05</v>
+      </c>
     </row>
     <row r="212">
       <c r="A212">
@@ -11703,6 +12973,12 @@
         <f>'Game'!E212/'Game'!G212</f>
         <v/>
       </c>
+      <c r="F212" t="n">
+        <v>0.2749784210684066</v>
+      </c>
+      <c r="G212" t="n">
+        <v>2.307661378506254e-06</v>
+      </c>
     </row>
     <row r="213">
       <c r="A213">
@@ -11725,6 +13001,12 @@
         <f>'Game'!E213/'Game'!G213</f>
         <v/>
       </c>
+      <c r="F213" t="n">
+        <v>0.6298815822625345</v>
+      </c>
+      <c r="G213" t="n">
+        <v>0.02519526329050139</v>
+      </c>
     </row>
     <row r="214">
       <c r="A214">
@@ -11747,6 +13029,12 @@
         <f>'Game'!E214/'Game'!G214</f>
         <v/>
       </c>
+      <c r="F214" t="n">
+        <v>0.1168821681642195</v>
+      </c>
+      <c r="G214" t="n">
+        <v>2.758456323705953e-05</v>
+      </c>
     </row>
     <row r="215">
       <c r="A215">
@@ -11769,6 +13057,12 @@
         <f>'Game'!E215/'Game'!G215</f>
         <v/>
       </c>
+      <c r="F215" t="n">
+        <v>0.1838047350397305</v>
+      </c>
+      <c r="G215" t="n">
+        <v>6.165979853585726e-05</v>
+      </c>
     </row>
     <row r="216">
       <c r="A216">
@@ -11791,6 +13085,12 @@
         <f>'Game'!E216/'Game'!G216</f>
         <v/>
       </c>
+      <c r="F216" t="n">
+        <v>0.224826158793367</v>
+      </c>
+      <c r="G216" t="n">
+        <v>4.650178404164229e-06</v>
+      </c>
     </row>
     <row r="217">
       <c r="A217">
@@ -11813,6 +13113,12 @@
         <f>'Game'!E217/'Game'!G217</f>
         <v/>
       </c>
+      <c r="F217" t="n">
+        <v>0.2931340100234243</v>
+      </c>
+      <c r="G217" t="n">
+        <v>3.298284763083948e-06</v>
+      </c>
     </row>
     <row r="218">
       <c r="A218">
@@ -11835,6 +13141,12 @@
         <f>'Game'!E218/'Game'!G218</f>
         <v/>
       </c>
+      <c r="F218" t="n">
+        <v>0.38387774875662</v>
+      </c>
+      <c r="G218" t="n">
+        <v>2.033450355961179e-05</v>
+      </c>
     </row>
     <row r="219">
       <c r="A219">
@@ -11857,6 +13169,12 @@
         <f>'Game'!E219/'Game'!G219</f>
         <v/>
       </c>
+      <c r="F219" t="n">
+        <v>0.3082993253485863</v>
+      </c>
+      <c r="G219" t="n">
+        <v>3.444200337137806e-06</v>
+      </c>
     </row>
     <row r="220">
       <c r="A220">
@@ -11879,6 +13197,12 @@
         <f>'Game'!E220/'Game'!G220</f>
         <v/>
       </c>
+      <c r="F220" t="n">
+        <v>0.3399943900925634</v>
+      </c>
+      <c r="G220" t="n">
+        <v>4.054633355959322e-06</v>
+      </c>
     </row>
     <row r="221">
       <c r="A221">
@@ -11901,6 +13225,12 @@
         <f>'Game'!E221/'Game'!G221</f>
         <v/>
       </c>
+      <c r="F221" t="n">
+        <v>0.05591452369129121</v>
+      </c>
+      <c r="G221" t="n">
+        <v>2.863196208159887e-05</v>
+      </c>
     </row>
     <row r="222">
       <c r="A222">
@@ -11923,6 +13253,12 @@
         <f>'Game'!E222/'Game'!G222</f>
         <v/>
       </c>
+      <c r="F222" t="n">
+        <v>0.2405279492274362</v>
+      </c>
+      <c r="G222" t="n">
+        <v>4.50188416457563e-05</v>
+      </c>
     </row>
     <row r="223">
       <c r="A223">
@@ -11945,6 +13281,12 @@
         <f>'Game'!E223/'Game'!G223</f>
         <v/>
       </c>
+      <c r="F223" t="n">
+        <v>0.1783350073046019</v>
+      </c>
+      <c r="G223" t="n">
+        <v>3.082410940662046e-06</v>
+      </c>
     </row>
     <row r="224">
       <c r="A224">
@@ -11967,6 +13309,12 @@
         <f>'Game'!E224/'Game'!G224</f>
         <v/>
       </c>
+      <c r="F224" t="n">
+        <v>0.5367038334071301</v>
+      </c>
+      <c r="G224" t="n">
+        <v>0.0002777777777777778</v>
+      </c>
     </row>
     <row r="225">
       <c r="A225">
@@ -11989,6 +13337,12 @@
         <f>'Game'!E225/'Game'!G225</f>
         <v/>
       </c>
+      <c r="F225" t="n">
+        <v>0.3704459687884453</v>
+      </c>
+      <c r="G225" t="n">
+        <v>5.034469441511564e-06</v>
+      </c>
     </row>
     <row r="226">
       <c r="A226">
@@ -12011,6 +13365,12 @@
         <f>'Game'!E226/'Game'!G226</f>
         <v/>
       </c>
+      <c r="F226" t="n">
+        <v>0.3052409877598364</v>
+      </c>
+      <c r="G226" t="n">
+        <v>0.0001348943305261823</v>
+      </c>
     </row>
     <row r="227">
       <c r="A227">
@@ -12033,6 +13393,12 @@
         <f>'Game'!E227/'Game'!G227</f>
         <v/>
       </c>
+      <c r="F227" t="n">
+        <v>0.3975517175029299</v>
+      </c>
+      <c r="G227" t="n">
+        <v>3.025605090762102e-05</v>
+      </c>
     </row>
     <row r="228">
       <c r="A228">
@@ -12055,6 +13421,12 @@
         <f>'Game'!E228/'Game'!G228</f>
         <v/>
       </c>
+      <c r="F228" t="n">
+        <v>0.133004121531718</v>
+      </c>
+      <c r="G228" t="n">
+        <v>1.150061191351811e-06</v>
+      </c>
     </row>
     <row r="229">
       <c r="A229">
@@ -12077,6 +13449,12 @@
         <f>'Game'!E229/'Game'!G229</f>
         <v/>
       </c>
+      <c r="F229" t="n">
+        <v>0.3386503056847303</v>
+      </c>
+      <c r="G229" t="n">
+        <v>2.176537308819872e-06</v>
+      </c>
     </row>
     <row r="230">
       <c r="A230">
@@ -12099,6 +13477,12 @@
         <f>'Game'!E230/'Game'!G230</f>
         <v/>
       </c>
+      <c r="F230" t="n">
+        <v>0.2698600101197504</v>
+      </c>
+      <c r="G230" t="n">
+        <v>6.615268675168081e-06</v>
+      </c>
     </row>
     <row r="231">
       <c r="A231">
@@ -12121,6 +13505,12 @@
         <f>'Game'!E231/'Game'!G231</f>
         <v/>
       </c>
+      <c r="F231" t="n">
+        <v>0.2517592305633691</v>
+      </c>
+      <c r="G231" t="n">
+        <v>2.485638487887239e-06</v>
+      </c>
     </row>
     <row r="232">
       <c r="A232">
@@ -12143,6 +13533,12 @@
         <f>'Game'!E232/'Game'!G232</f>
         <v/>
       </c>
+      <c r="F232" t="n">
+        <v>0.3138510306083218</v>
+      </c>
+      <c r="G232" t="n">
+        <v>0.0001110369630946446</v>
+      </c>
     </row>
     <row r="233">
       <c r="A233">
@@ -12165,6 +13561,12 @@
         <f>'Game'!E233/'Game'!G233</f>
         <v/>
       </c>
+      <c r="F233" t="n">
+        <v>0.3127987227802551</v>
+      </c>
+      <c r="G233" t="n">
+        <v>2.761323463730103e-06</v>
+      </c>
     </row>
     <row r="234">
       <c r="A234">
@@ -12187,6 +13589,12 @@
         <f>'Game'!E234/'Game'!G234</f>
         <v/>
       </c>
+      <c r="F234" t="n">
+        <v>0.2218810095257972</v>
+      </c>
+      <c r="G234" t="n">
+        <v>3.45669010146721e-06</v>
+      </c>
     </row>
     <row r="235">
       <c r="A235">
@@ -12209,6 +13617,12 @@
         <f>'Game'!E235/'Game'!G235</f>
         <v/>
       </c>
+      <c r="F235" t="n">
+        <v>0.2099560269565971</v>
+      </c>
+      <c r="G235" t="n">
+        <v>1.500753186597312e-06</v>
+      </c>
     </row>
     <row r="236">
       <c r="A236">
@@ -12231,6 +13645,12 @@
         <f>'Game'!E236/'Game'!G236</f>
         <v/>
       </c>
+      <c r="F236" t="n">
+        <v>0.1154960301848875</v>
+      </c>
+      <c r="G236" t="n">
+        <v>0.0001360770897124785</v>
+      </c>
     </row>
     <row r="237">
       <c r="A237">
@@ -12253,6 +13673,12 @@
         <f>'Game'!E237/'Game'!G237</f>
         <v/>
       </c>
+      <c r="F237" t="n">
+        <v>0.1857907253269917</v>
+      </c>
+      <c r="G237" t="n">
+        <v>0.0008818298410115913</v>
+      </c>
     </row>
     <row r="238">
       <c r="A238">
@@ -12275,6 +13701,12 @@
         <f>'Game'!E238/'Game'!G238</f>
         <v/>
       </c>
+      <c r="F238" t="n">
+        <v>0.2064030296906936</v>
+      </c>
+      <c r="G238" t="n">
+        <v>2.183702067620995e-06</v>
+      </c>
     </row>
     <row r="239">
       <c r="A239">
@@ -12297,6 +13729,12 @@
         <f>'Game'!E239/'Game'!G239</f>
         <v/>
       </c>
+      <c r="F239" t="n">
+        <v>0.058627300388699</v>
+      </c>
+      <c r="G239" t="n">
+        <v>4.829166939193157e-06</v>
+      </c>
     </row>
     <row r="240">
       <c r="A240">
@@ -12319,6 +13757,12 @@
         <f>'Game'!E240/'Game'!G240</f>
         <v/>
       </c>
+      <c r="F240" t="n">
+        <v>0.2832346874122857</v>
+      </c>
+      <c r="G240" t="n">
+        <v>3.052967312284422e-06</v>
+      </c>
     </row>
     <row r="241">
       <c r="A241">
@@ -12341,6 +13785,12 @@
         <f>'Game'!E241/'Game'!G241</f>
         <v/>
       </c>
+      <c r="F241" t="n">
+        <v>0.0979008491528052</v>
+      </c>
+      <c r="G241" t="n">
+        <v>8.265965644448037e-07</v>
+      </c>
     </row>
     <row r="242">
       <c r="A242">
@@ -12363,6 +13813,12 @@
         <f>'Game'!E242/'Game'!G242</f>
         <v/>
       </c>
+      <c r="F242" t="n">
+        <v>0.1804758804391302</v>
+      </c>
+      <c r="G242" t="n">
+        <v>1.102073504215267e-06</v>
+      </c>
     </row>
     <row r="243">
       <c r="A243">
@@ -12385,6 +13841,12 @@
         <f>'Game'!E243/'Game'!G243</f>
         <v/>
       </c>
+      <c r="F243" t="n">
+        <v>0.09121822948882854</v>
+      </c>
+      <c r="G243" t="n">
+        <v>2.709285945364584e-05</v>
+      </c>
     </row>
     <row r="244">
       <c r="A244">
@@ -12407,6 +13869,12 @@
         <f>'Game'!E244/'Game'!G244</f>
         <v/>
       </c>
+      <c r="F244" t="n">
+        <v>0.06746500252993759</v>
+      </c>
+      <c r="G244" t="n">
+        <v>4.849434749885554e-05</v>
+      </c>
     </row>
     <row r="245">
       <c r="A245">
@@ -12429,6 +13897,12 @@
         <f>'Game'!E245/'Game'!G245</f>
         <v/>
       </c>
+      <c r="F245" t="n">
+        <v>0.5160853481305325</v>
+      </c>
+      <c r="G245" t="n">
+        <v>2.399157093582022e-05</v>
+      </c>
     </row>
     <row r="246">
       <c r="A246">
@@ -12451,6 +13925,12 @@
         <f>'Game'!E246/'Game'!G246</f>
         <v/>
       </c>
+      <c r="F246" t="n">
+        <v>0.05497458112805093</v>
+      </c>
+      <c r="G246" t="n">
+        <v>4.842885929946607e-06</v>
+      </c>
     </row>
     <row r="247">
       <c r="A247">
@@ -12473,6 +13953,12 @@
         <f>'Game'!E247/'Game'!G247</f>
         <v/>
       </c>
+      <c r="F247" t="n">
+        <v>0.4162330905306971</v>
+      </c>
+      <c r="G247" t="n">
+        <v>4.435568871133309e-05</v>
+      </c>
     </row>
     <row r="248">
       <c r="A248">
@@ -12495,6 +13981,12 @@
         <f>'Game'!E248/'Game'!G248</f>
         <v/>
       </c>
+      <c r="F248" t="n">
+        <v>0.4156965348783943</v>
+      </c>
+      <c r="G248" t="n">
+        <v>4.834609834706431e-05</v>
+      </c>
     </row>
     <row r="249">
       <c r="A249">
@@ -12517,6 +14009,12 @@
         <f>'Game'!E249/'Game'!G249</f>
         <v/>
       </c>
+      <c r="F249" t="n">
+        <v>0.09963906744209773</v>
+      </c>
+      <c r="G249" t="n">
+        <v>2.296519135815513e-06</v>
+      </c>
     </row>
     <row r="250">
       <c r="A250">
@@ -12539,6 +14037,12 @@
         <f>'Game'!E250/'Game'!G250</f>
         <v/>
       </c>
+      <c r="F250" t="n">
+        <v>0.1125320026949164</v>
+      </c>
+      <c r="G250" t="n">
+        <v>1.523593556599438e-06</v>
+      </c>
     </row>
     <row r="251">
       <c r="A251">
@@ -12561,6 +14065,12 @@
         <f>'Game'!E251/'Game'!G251</f>
         <v/>
       </c>
+      <c r="F251" t="n">
+        <v>0.04084516154751533</v>
+      </c>
+      <c r="G251" t="n">
+        <v>1.888275726814705e-06</v>
+      </c>
     </row>
     <row r="252">
       <c r="A252">
@@ -12582,6 +14092,12 @@
       <c r="E252">
         <f>'Game'!E252/'Game'!G252</f>
         <v/>
+      </c>
+      <c r="F252" t="n">
+        <v>0.06932503207669234</v>
+      </c>
+      <c r="G252" t="n">
+        <v>8.217646294911131e-06</v>
       </c>
     </row>
   </sheetData>

</xml_diff>